<commit_message>
Replaced the New Jar File with Extent Reports extension
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_Demo.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_Demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/03-Aug-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ideyalabs/Documents/16-AUg-2023_v3.0_Android/coyni-automation/Mobile/coyni_mobile/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D18EA6-5C03-5241-BDF9-6F3502CA96E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3219865-2FDA-D340-A21C-9484D9D2B90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -82,19 +82,7 @@
     <t>Keywords8</t>
   </si>
   <si>
-    <t>Verify SignUp with valid credentials</t>
-  </si>
-  <si>
-    <t>testdata_3_0_customer.xls,SignupPage</t>
-  </si>
-  <si>
     <t>RunRangeOfIterations</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>SignUp</t>
   </si>
   <si>
     <t xml:space="preserve">coyni_mobile.tests.SignUpTest,
@@ -145,9 +133,6 @@
 </t>
   </si>
   <si>
-    <t>testdata_3_0_customer.xls,buyTokens</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -164,15 +149,6 @@
 -pcardHeading,
 -premovePopUpHeading,
 -ptoastMsg</t>
-  </si>
-  <si>
-    <t>Verify Buy Token with New and Existing Debit and Credit Cards</t>
-  </si>
-  <si>
-    <t>Verify Send Transaction</t>
-  </si>
-  <si>
-    <t>testdata_3_0_customer.xls,notifications</t>
   </si>
   <si>
     <t>coyni_mobile.tests.DashBoardTest,
@@ -197,9 +173,6 @@
 -ppin</t>
   </si>
   <si>
-    <t>Verify Request Transaction</t>
-  </si>
-  <si>
     <t>coyni_mobile.tests.DashBoardTest,
 testRequest,
 -pname,
@@ -216,12 +189,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Send</t>
-  </si>
-  <si>
-    <t>Request</t>
   </si>
   <si>
     <t xml:space="preserve">coyni_mobile.tests.DashBoardTest,
@@ -254,9 +221,6 @@
 </t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>coyni_mobile.tests.DashBoardTest,
 verifySentTransaction,
 -pname,
@@ -266,21 +230,6 @@
 -ptransDtlsHeading,
 -ptransactionType1,
 -ptransactionStatus</t>
-  </si>
-  <si>
-    <t>Buy Tokens - Credit Card</t>
-  </si>
-  <si>
-    <t>Verify Add Debit and Credit Card invalid data</t>
-  </si>
-  <si>
-    <t>testdata_3_0_customer.xls,PaymentMethods</t>
-  </si>
-  <si>
-    <t>Verify Withdraw Token with Gift Cards</t>
-  </si>
-  <si>
-    <t>Withdraw Token - Gift Card</t>
   </si>
   <si>
     <t>coyni_mobile.tests.DashBoardTest,
@@ -301,12 +250,6 @@
 -ptransactionStatus</t>
   </si>
   <si>
-    <t>Verify Scan Code and My QR Code</t>
-  </si>
-  <si>
-    <t>Scan Code</t>
-  </si>
-  <si>
     <t>coyni_mobile.tests.DashBoardTest,
 testMyQRCode,
 -pamount,
@@ -330,12 +273,6 @@
 -pmessage,
 -perrorMessage,
 -psendErrMsg</t>
-  </si>
-  <si>
-    <t>Verify Filters with one Transactions Type</t>
-  </si>
-  <si>
-    <t>testdata_3_0_customer.xls,filters</t>
   </si>
   <si>
     <t>Filters</t>
@@ -376,10 +313,64 @@
 </t>
   </si>
   <si>
-    <t>Payment Methods - Debit Card</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>TC_01.Verify SignUp with valid credentials</t>
+  </si>
+  <si>
+    <t>Add Credit Card and Do Buy Tokens</t>
+  </si>
+  <si>
+    <t>Do Withdraw Tokens with Gift Card</t>
+  </si>
+  <si>
+    <t>Add Card flow verify error messages</t>
+  </si>
+  <si>
+    <t>Send Tokens from One User To another User</t>
+  </si>
+  <si>
+    <t>Request Tokens From one User to Another User</t>
+  </si>
+  <si>
+    <t>Verify Scan Code</t>
+  </si>
+  <si>
+    <t>Complete Sign Up flow and Add Address,Payment Method</t>
+  </si>
+  <si>
+    <t>testdata_Demo.xlsx,SignupPage</t>
+  </si>
+  <si>
+    <t>testdata_Demo.xlsx,buyTokens</t>
+  </si>
+  <si>
+    <t>testdata_Demo.xlsx,PaymentMethods</t>
+  </si>
+  <si>
+    <t>testdata_Demo.xlsx,notifications</t>
+  </si>
+  <si>
+    <t>testdata_Demo.xlsx,filters</t>
+  </si>
+  <si>
+    <t>TC_02.Verify Buy Token with New and Existing Debit and Credit Cards</t>
+  </si>
+  <si>
+    <t>TC_03.Verify Withdraw Token with Gift Cards</t>
+  </si>
+  <si>
+    <t>TC_04.Verify Add Debit and Credit Card invalid data</t>
+  </si>
+  <si>
+    <t>TC_05.Verify Scan Code and My QR Code</t>
+  </si>
+  <si>
+    <t>TC_06.Verify Send Transaction</t>
+  </si>
+  <si>
+    <t>TC_07.Verify Request Transaction</t>
+  </si>
+  <si>
+    <t>TC_08.Verify Filters with one Transactions Type</t>
   </si>
 </sst>
 </file>
@@ -823,251 +814,251 @@
     </row>
     <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:15" ht="384" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="224" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="280" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:15" ht="224" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="J6" s="10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="208" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="I8" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:15" ht="176" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>

</xml_diff>